<commit_message>
Adding BrowserStack and ending TestRail
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codebase\UISpiceJet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB95A458-48E6-40DF-A760-658141830EE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46216950-5086-400E-BC29-1AE9825EEA59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACC7127D-CA10-4415-AB1E-B8CD0C7426B6}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>arrival</t>
   </si>
   <si>
-    <t>Test_1</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -75,13 +72,16 @@
     <t>CHIHUAHUA</t>
   </si>
   <si>
-    <t>Test_2</t>
-  </si>
-  <si>
     <t>Mexico</t>
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>Test_01</t>
+  </si>
+  <si>
+    <t>Test_02</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +461,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -482,21 +482,21 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -516,16 +516,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>

</xml_diff>